<commit_message>
Auto commit Tue Jun 21 16:10:01 IST 2022
</commit_message>
<xml_diff>
--- a/temp_files/source-prediction-counts.xlsx
+++ b/temp_files/source-prediction-counts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
   <si>
     <t>class</t>
   </si>
@@ -25,12 +25,21 @@
     <t>variable sources</t>
   </si>
   <si>
+    <t>All Sources</t>
+  </si>
+  <si>
     <t>Argmax</t>
   </si>
   <si>
     <t>4-sigma</t>
   </si>
   <si>
+    <t>argmax</t>
+  </si>
+  <si>
+    <t>3-sigma</t>
+  </si>
+  <si>
     <t>AGN</t>
   </si>
   <si>
@@ -56,6 +65,9 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -700,7 +712,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -769,9 +781,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
@@ -1107,10 +1116,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="K1" sqref="K1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="15.75"/>
@@ -1121,7 +1130,7 @@
     <col min="10" max="11" width="8.11111111111111" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22" customHeight="1" spans="1:9">
+    <row r="1" ht="22" customHeight="1" spans="1:14">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1132,11 +1141,17 @@
         <v>2</v>
       </c>
       <c r="I1" s="3"/>
+      <c r="K1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="27" customHeight="1" spans="1:12">
+    <row r="2" s="1" customFormat="1" ht="27" customHeight="1" spans="1:14">
       <c r="A2" s="6"/>
       <c r="B2" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="8">
         <v>0.9</v>
@@ -1145,10 +1160,10 @@
         <v>0.997</v>
       </c>
       <c r="E2" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>4</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>3</v>
       </c>
       <c r="G2" s="8">
         <v>0.9</v>
@@ -1157,15 +1172,25 @@
         <v>0.997</v>
       </c>
       <c r="I2" s="18" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J2" s="19"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="21"/>
+      <c r="K2" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="21">
+        <v>0.9</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:14">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B3" s="9">
         <v>103705</v>
@@ -1192,11 +1217,26 @@
         <v>1031</v>
       </c>
       <c r="J3" s="23"/>
-      <c r="L3" s="24"/>
+      <c r="K3">
+        <f>SUM(B3,F3)</f>
+        <v>114642</v>
+      </c>
+      <c r="L3">
+        <f>SUM(C3,G3)</f>
+        <v>107017</v>
+      </c>
+      <c r="M3">
+        <f>SUM(D3,H3)</f>
+        <v>32600</v>
+      </c>
+      <c r="N3">
+        <f>SUM(E3,I3)</f>
+        <v>8574</v>
+      </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:14">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B4" s="9">
         <v>54456</v>
@@ -1223,11 +1263,26 @@
         <v>1153</v>
       </c>
       <c r="J4" s="23"/>
-      <c r="L4" s="24"/>
+      <c r="K4">
+        <f t="shared" ref="K4:K10" si="0">SUM(B4,F4)</f>
+        <v>63967</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L10" si="1">SUM(C4,G4)</f>
+        <v>55763</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M10" si="2">SUM(D4,H4)</f>
+        <v>16148</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ref="N4:N10" si="3">SUM(E4,I4)</f>
+        <v>5166</v>
+      </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:14">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" s="9">
         <v>31715</v>
@@ -1254,11 +1309,26 @@
         <v>153</v>
       </c>
       <c r="J5" s="23"/>
-      <c r="L5" s="24"/>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>40524</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>39418</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="2"/>
+        <v>5184</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="3"/>
+        <v>208</v>
+      </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:14">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B6" s="9">
         <v>20112</v>
@@ -1285,11 +1355,26 @@
         <v>46</v>
       </c>
       <c r="J6" s="23"/>
-      <c r="L6" s="24"/>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>23142</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="1"/>
+        <v>18052</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="2"/>
+        <v>362</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:14">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" s="9">
         <v>8726</v>
@@ -1316,11 +1401,26 @@
         <v>0</v>
       </c>
       <c r="J7" s="23"/>
-      <c r="L7" s="24"/>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>10999</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="1"/>
+        <v>7570</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="2"/>
+        <v>79</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:14">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B8" s="9">
         <v>6530</v>
@@ -1347,11 +1447,26 @@
         <v>1</v>
       </c>
       <c r="J8" s="23"/>
-      <c r="L8" s="24"/>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>8321</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="1"/>
+        <v>6245</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="2"/>
+        <v>173</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:14">
       <c r="A9" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9" s="9">
         <v>4703</v>
@@ -1378,11 +1493,26 @@
         <v>0</v>
       </c>
       <c r="J9" s="23"/>
-      <c r="L9" s="24"/>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>6083</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="1"/>
+        <v>4406</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="N9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:14">
       <c r="A10" s="10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B10" s="11">
         <v>1546</v>
@@ -1408,8 +1538,23 @@
       <c r="I10" s="22">
         <v>43</v>
       </c>
-      <c r="J10" s="25"/>
-      <c r="L10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>1688</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="1"/>
+        <v>1120</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="2"/>
+        <v>197</v>
+      </c>
+      <c r="N10">
+        <f t="shared" si="3"/>
+        <v>71</v>
+      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11" s="13"/>
@@ -1419,7 +1564,7 @@
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="14" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B12" s="15">
         <f>SUM(B3:B10)</f>
@@ -1449,19 +1594,55 @@
         <f>SUM(H3:H10)</f>
         <v>9373</v>
       </c>
-      <c r="I12" s="26">
+      <c r="I12" s="25">
         <f>SUM(I3:I10)</f>
         <v>2427</v>
       </c>
-      <c r="J12" s="27"/>
+      <c r="J12" s="26"/>
     </row>
     <row r="13" spans="9:9">
-      <c r="I13" s="28"/>
+      <c r="I13" s="27"/>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="3">
+        <f>SUM(B12,F12)</f>
+        <v>269366</v>
+      </c>
+      <c r="C15" s="3">
+        <f>SUM(C12,G12)</f>
+        <v>239591</v>
+      </c>
+      <c r="D15" s="3">
+        <f>SUM(D12,H12)</f>
+        <v>54770</v>
+      </c>
+      <c r="E15" s="3">
+        <f>SUM(E12,I12)</f>
+        <v>14066</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:I1"/>
+    <mergeCell ref="K1:N1"/>
     <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Auto commit Wed Jun 22 11:00:02 IST 2022
</commit_message>
<xml_diff>
--- a/temp_files/source-prediction-counts.xlsx
+++ b/temp_files/source-prediction-counts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>class</t>
   </si>
@@ -66,9 +66,6 @@
   <si>
     <t>TOTAL</t>
   </si>
-  <si>
-    <t>Total</t>
-  </si>
 </sst>
 </file>
 
@@ -427,7 +424,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -436,9 +433,31 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -453,6 +472,61 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -597,7 +671,7 @@
     <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -639,10 +713,10 @@
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -651,28 +725,28 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -693,13 +767,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -712,7 +786,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -725,77 +799,89 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1116,39 +1202,39 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:N1"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="8.11111111111111" style="2" customWidth="1"/>
-    <col min="2" max="8" width="8.11111111111111" style="3" customWidth="1"/>
-    <col min="9" max="9" width="8.11111111111111" style="4" customWidth="1"/>
-    <col min="10" max="11" width="8.11111111111111" customWidth="1"/>
+    <col min="2" max="11" width="8.11111111111111" style="3" customWidth="1"/>
+    <col min="12" max="12" width="8" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22" customHeight="1" spans="1:14">
-      <c r="A1" s="5" t="s">
+    <row r="1" ht="22" customHeight="1" spans="1:13">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="E1" s="15"/>
       <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="K1" s="3" t="s">
+      <c r="I1" s="15"/>
+      <c r="J1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
     </row>
-    <row r="2" s="1" customFormat="1" ht="27" customHeight="1" spans="1:14">
+    <row r="2" s="1" customFormat="1" ht="27" customHeight="1" spans="1:13">
       <c r="A2" s="6"/>
       <c r="B2" s="7" t="s">
         <v>4</v>
@@ -1162,7 +1248,7 @@
       <c r="E2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="17" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="8">
@@ -1171,28 +1257,27 @@
       <c r="H2" s="8">
         <v>0.997</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="20" t="s">
+      <c r="J2" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="21">
+      <c r="K2" s="23">
         <v>0.9</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="L2" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="M2" s="30" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:13">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="5">
         <v>103705</v>
       </c>
       <c r="C3" s="3">
@@ -1201,10 +1286,10 @@
       <c r="D3" s="3">
         <v>29063</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="15">
         <v>7543</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="18">
         <v>10937</v>
       </c>
       <c r="G3" s="3">
@@ -1213,32 +1298,31 @@
       <c r="H3" s="3">
         <v>3537</v>
       </c>
-      <c r="I3" s="22">
+      <c r="I3" s="25">
         <v>1031</v>
       </c>
-      <c r="J3" s="23"/>
-      <c r="K3">
+      <c r="J3" s="26">
         <f>SUM(B3,F3)</f>
         <v>114642</v>
       </c>
-      <c r="L3">
+      <c r="K3" s="3">
         <f>SUM(C3,G3)</f>
         <v>107017</v>
       </c>
-      <c r="M3">
+      <c r="L3" s="3">
         <f>SUM(D3,H3)</f>
         <v>32600</v>
       </c>
-      <c r="N3">
+      <c r="M3">
         <f>SUM(E3,I3)</f>
         <v>8574</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:13">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="5">
         <v>54456</v>
       </c>
       <c r="C4" s="3">
@@ -1247,10 +1331,10 @@
       <c r="D4" s="3">
         <v>12652</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="15">
         <v>4013</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="18">
         <v>9511</v>
       </c>
       <c r="G4" s="3">
@@ -1259,32 +1343,31 @@
       <c r="H4" s="3">
         <v>3496</v>
       </c>
-      <c r="I4" s="22">
+      <c r="I4" s="25">
         <v>1153</v>
       </c>
-      <c r="J4" s="23"/>
-      <c r="K4">
-        <f t="shared" ref="K4:K10" si="0">SUM(B4,F4)</f>
+      <c r="J4" s="3">
+        <f t="shared" ref="J4:J10" si="0">SUM(B4,F4)</f>
         <v>63967</v>
       </c>
-      <c r="L4">
-        <f t="shared" ref="L4:L10" si="1">SUM(C4,G4)</f>
+      <c r="K4" s="3">
+        <f t="shared" ref="K4:K10" si="1">SUM(C4,G4)</f>
         <v>55763</v>
       </c>
+      <c r="L4" s="3">
+        <f t="shared" ref="L4:L10" si="2">SUM(D4,H4)</f>
+        <v>16148</v>
+      </c>
       <c r="M4">
-        <f t="shared" ref="M4:M10" si="2">SUM(D4,H4)</f>
-        <v>16148</v>
-      </c>
-      <c r="N4">
-        <f t="shared" ref="N4:N10" si="3">SUM(E4,I4)</f>
+        <f t="shared" ref="M4:M10" si="3">SUM(E4,I4)</f>
         <v>5166</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:13">
       <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="5">
         <v>31715</v>
       </c>
       <c r="C5" s="3">
@@ -1293,10 +1376,10 @@
       <c r="D5" s="3">
         <v>3311</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="15">
         <v>55</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="18">
         <v>8809</v>
       </c>
       <c r="G5" s="3">
@@ -1305,32 +1388,31 @@
       <c r="H5" s="3">
         <v>1873</v>
       </c>
-      <c r="I5" s="22">
+      <c r="I5" s="25">
         <v>153</v>
       </c>
-      <c r="J5" s="23"/>
-      <c r="K5">
+      <c r="J5" s="3">
         <f t="shared" si="0"/>
         <v>40524</v>
       </c>
-      <c r="L5">
+      <c r="K5" s="3">
         <f t="shared" si="1"/>
         <v>39418</v>
       </c>
-      <c r="M5">
+      <c r="L5" s="3">
         <f t="shared" si="2"/>
         <v>5184</v>
       </c>
-      <c r="N5">
+      <c r="M5">
         <f t="shared" si="3"/>
         <v>208</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:13">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="5">
         <v>20112</v>
       </c>
       <c r="C6" s="3">
@@ -1339,10 +1421,10 @@
       <c r="D6" s="3">
         <v>52</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="15">
         <v>0</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="18">
         <v>3030</v>
       </c>
       <c r="G6" s="3">
@@ -1351,32 +1433,31 @@
       <c r="H6" s="3">
         <v>310</v>
       </c>
-      <c r="I6" s="22">
+      <c r="I6" s="25">
         <v>46</v>
       </c>
-      <c r="J6" s="23"/>
-      <c r="K6">
+      <c r="J6" s="3">
         <f t="shared" si="0"/>
         <v>23142</v>
       </c>
-      <c r="L6">
+      <c r="K6" s="3">
         <f t="shared" si="1"/>
         <v>18052</v>
       </c>
-      <c r="M6">
+      <c r="L6" s="3">
         <f t="shared" si="2"/>
         <v>362</v>
       </c>
-      <c r="N6">
+      <c r="M6">
         <f t="shared" si="3"/>
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:13">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="5">
         <v>8726</v>
       </c>
       <c r="C7" s="3">
@@ -1385,10 +1466,10 @@
       <c r="D7" s="3">
         <v>45</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="15">
         <v>0</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="18">
         <v>2273</v>
       </c>
       <c r="G7" s="3">
@@ -1397,32 +1478,31 @@
       <c r="H7" s="3">
         <v>34</v>
       </c>
-      <c r="I7" s="22">
+      <c r="I7" s="25">
         <v>0</v>
       </c>
-      <c r="J7" s="23"/>
-      <c r="K7">
+      <c r="J7" s="3">
         <f t="shared" si="0"/>
         <v>10999</v>
       </c>
-      <c r="L7">
+      <c r="K7" s="3">
         <f t="shared" si="1"/>
         <v>7570</v>
       </c>
-      <c r="M7">
+      <c r="L7" s="3">
         <f t="shared" si="2"/>
         <v>79</v>
       </c>
-      <c r="N7">
+      <c r="M7">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:13">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="5">
         <v>6530</v>
       </c>
       <c r="C8" s="3">
@@ -1431,10 +1511,10 @@
       <c r="D8" s="3">
         <v>129</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="15">
         <v>0</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="18">
         <v>1791</v>
       </c>
       <c r="G8" s="3">
@@ -1443,32 +1523,31 @@
       <c r="H8" s="3">
         <v>44</v>
       </c>
-      <c r="I8" s="22">
+      <c r="I8" s="25">
         <v>1</v>
       </c>
-      <c r="J8" s="23"/>
-      <c r="K8">
+      <c r="J8" s="3">
         <f t="shared" si="0"/>
         <v>8321</v>
       </c>
-      <c r="L8">
+      <c r="K8" s="3">
         <f t="shared" si="1"/>
         <v>6245</v>
       </c>
-      <c r="M8">
+      <c r="L8" s="3">
         <f t="shared" si="2"/>
         <v>173</v>
       </c>
-      <c r="N8">
+      <c r="M8">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:13">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="5">
         <v>4703</v>
       </c>
       <c r="C9" s="3">
@@ -1477,10 +1556,10 @@
       <c r="D9" s="3">
         <v>16</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="15">
         <v>0</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="18">
         <v>1380</v>
       </c>
       <c r="G9" s="3">
@@ -1489,44 +1568,43 @@
       <c r="H9" s="3">
         <v>11</v>
       </c>
-      <c r="I9" s="22">
+      <c r="I9" s="25">
         <v>0</v>
       </c>
-      <c r="J9" s="23"/>
-      <c r="K9">
+      <c r="J9" s="3">
         <f t="shared" si="0"/>
         <v>6083</v>
       </c>
-      <c r="L9">
+      <c r="K9" s="3">
         <f t="shared" si="1"/>
         <v>4406</v>
       </c>
-      <c r="M9">
+      <c r="L9" s="3">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="N9">
+      <c r="M9">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:13">
+      <c r="A10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="11">
+      <c r="B10" s="10">
         <v>1546</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <v>984</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="11">
         <v>129</v>
       </c>
-      <c r="E10" s="12">
+      <c r="E10" s="19">
         <v>28</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="18">
         <v>142</v>
       </c>
       <c r="G10" s="3">
@@ -1535,114 +1613,90 @@
       <c r="H10" s="3">
         <v>68</v>
       </c>
-      <c r="I10" s="22">
+      <c r="I10" s="25">
         <v>43</v>
       </c>
-      <c r="J10" s="24"/>
-      <c r="K10">
+      <c r="J10" s="3">
         <f t="shared" si="0"/>
         <v>1688</v>
       </c>
-      <c r="L10">
+      <c r="K10" s="3">
         <f t="shared" si="1"/>
         <v>1120</v>
       </c>
-      <c r="M10">
+      <c r="L10" s="3">
         <f t="shared" si="2"/>
         <v>197</v>
       </c>
-      <c r="N10">
+      <c r="M10">
         <f t="shared" si="3"/>
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="13"/>
-      <c r="F11" s="9"/>
-      <c r="I11" s="22"/>
-      <c r="J11" s="23"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="14" t="s">
+    <row r="11" spans="1:13">
+      <c r="A11" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B11" s="13">
         <f>SUM(B3:B10)</f>
         <v>231493</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C11" s="14">
         <f>SUM(C3:C10)</f>
         <v>204180</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D11" s="14">
         <f>SUM(D3:D10)</f>
         <v>45397</v>
       </c>
-      <c r="E12" s="15">
+      <c r="E11" s="20">
         <f>SUM(E3:E10)</f>
         <v>11639</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F11" s="21">
         <f>SUM(F3:F10)</f>
         <v>37873</v>
       </c>
-      <c r="G12" s="15">
+      <c r="G11" s="14">
         <f>SUM(G3:G10)</f>
         <v>35411</v>
       </c>
-      <c r="H12" s="15">
+      <c r="H11" s="14">
         <f>SUM(H3:H10)</f>
         <v>9373</v>
       </c>
-      <c r="I12" s="25">
+      <c r="I11" s="27">
         <f>SUM(I3:I10)</f>
         <v>2427</v>
       </c>
-      <c r="J12" s="26"/>
+      <c r="J11" s="14">
+        <f>SUM(J3:J10)</f>
+        <v>269366</v>
+      </c>
+      <c r="K11" s="14">
+        <f>SUM(K3:K10)</f>
+        <v>239591</v>
+      </c>
+      <c r="L11" s="14">
+        <f>SUM(L3:L10)</f>
+        <v>54770</v>
+      </c>
+      <c r="M11" s="31">
+        <f>SUM(M3:M10)</f>
+        <v>14066</v>
+      </c>
+    </row>
+    <row r="12" spans="9:9">
+      <c r="I12" s="28"/>
     </row>
     <row r="13" spans="9:9">
-      <c r="I13" s="27"/>
-    </row>
-    <row r="14" spans="2:5">
-      <c r="B14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="3">
-        <f>SUM(B12,F12)</f>
-        <v>269366</v>
-      </c>
-      <c r="C15" s="3">
-        <f>SUM(C12,G12)</f>
-        <v>239591</v>
-      </c>
-      <c r="D15" s="3">
-        <f>SUM(D12,H12)</f>
-        <v>54770</v>
-      </c>
-      <c r="E15" s="3">
-        <f>SUM(E12,I12)</f>
-        <v>14066</v>
-      </c>
+      <c r="I13" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:I1"/>
-    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="J1:M1"/>
     <mergeCell ref="A1:A2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Auto commit Mon Jul  4 14:50:01 IST 2022
</commit_message>
<xml_diff>
--- a/temp_files/source-prediction-counts.xlsx
+++ b/temp_files/source-prediction-counts.xlsx
@@ -73,11 +73,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,8 +86,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -109,43 +133,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -154,6 +141,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -161,40 +156,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -208,23 +186,53 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -239,187 +247,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -536,6 +544,21 @@
         <color auto="1"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -544,24 +567,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -581,17 +586,46 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -610,183 +644,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -817,9 +825,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -838,43 +843,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
@@ -1205,7 +1186,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="15.75"/>
@@ -1222,17 +1203,17 @@
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="15"/>
+      <c r="E1" s="14"/>
       <c r="F1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="15"/>
-      <c r="J1" s="14" t="s">
+      <c r="I1" s="14"/>
+      <c r="J1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
     </row>
     <row r="2" s="1" customFormat="1" ht="27" customHeight="1" spans="1:13">
       <c r="A2" s="6"/>
@@ -1245,10 +1226,10 @@
       <c r="D2" s="8">
         <v>0.997</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="F2" s="8" t="s">
         <v>4</v>
       </c>
       <c r="G2" s="8">
@@ -1257,19 +1238,19 @@
       <c r="H2" s="8">
         <v>0.997</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="23">
+      <c r="K2" s="17">
         <v>0.9</v>
       </c>
-      <c r="L2" s="24" t="s">
+      <c r="L2" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="M2" s="30" t="s">
+      <c r="M2" s="21" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1286,10 +1267,10 @@
       <c r="D3" s="3">
         <v>29063</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E3" s="14">
         <v>7543</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="10">
         <v>10937</v>
       </c>
       <c r="G3" s="3">
@@ -1298,10 +1279,10 @@
       <c r="H3" s="3">
         <v>3537</v>
       </c>
-      <c r="I3" s="25">
+      <c r="I3" s="14">
         <v>1031</v>
       </c>
-      <c r="J3" s="26">
+      <c r="J3" s="18">
         <f>SUM(B3,F3)</f>
         <v>114642</v>
       </c>
@@ -1309,7 +1290,7 @@
         <f>SUM(C3,G3)</f>
         <v>107017</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3" s="19">
         <f>SUM(D3,H3)</f>
         <v>32600</v>
       </c>
@@ -1331,10 +1312,10 @@
       <c r="D4" s="3">
         <v>12652</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="14">
         <v>4013</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="10">
         <v>9511</v>
       </c>
       <c r="G4" s="3">
@@ -1343,7 +1324,7 @@
       <c r="H4" s="3">
         <v>3496</v>
       </c>
-      <c r="I4" s="25">
+      <c r="I4" s="14">
         <v>1153</v>
       </c>
       <c r="J4" s="3">
@@ -1354,7 +1335,7 @@
         <f t="shared" ref="K4:K10" si="1">SUM(C4,G4)</f>
         <v>55763</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4" s="19">
         <f t="shared" ref="L4:L10" si="2">SUM(D4,H4)</f>
         <v>16148</v>
       </c>
@@ -1376,10 +1357,10 @@
       <c r="D5" s="3">
         <v>3311</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="14">
         <v>55</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="10">
         <v>8809</v>
       </c>
       <c r="G5" s="3">
@@ -1388,7 +1369,7 @@
       <c r="H5" s="3">
         <v>1873</v>
       </c>
-      <c r="I5" s="25">
+      <c r="I5" s="14">
         <v>153</v>
       </c>
       <c r="J5" s="3">
@@ -1399,7 +1380,7 @@
         <f t="shared" si="1"/>
         <v>39418</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5" s="19">
         <f t="shared" si="2"/>
         <v>5184</v>
       </c>
@@ -1421,10 +1402,10 @@
       <c r="D6" s="3">
         <v>52</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <v>0</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="10">
         <v>3030</v>
       </c>
       <c r="G6" s="3">
@@ -1433,7 +1414,7 @@
       <c r="H6" s="3">
         <v>310</v>
       </c>
-      <c r="I6" s="25">
+      <c r="I6" s="14">
         <v>46</v>
       </c>
       <c r="J6" s="3">
@@ -1444,7 +1425,7 @@
         <f t="shared" si="1"/>
         <v>18052</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6" s="19">
         <f t="shared" si="2"/>
         <v>362</v>
       </c>
@@ -1466,10 +1447,10 @@
       <c r="D7" s="3">
         <v>45</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <v>0</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="10">
         <v>2273</v>
       </c>
       <c r="G7" s="3">
@@ -1478,7 +1459,7 @@
       <c r="H7" s="3">
         <v>34</v>
       </c>
-      <c r="I7" s="25">
+      <c r="I7" s="14">
         <v>0</v>
       </c>
       <c r="J7" s="3">
@@ -1489,7 +1470,7 @@
         <f t="shared" si="1"/>
         <v>7570</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="19">
         <f t="shared" si="2"/>
         <v>79</v>
       </c>
@@ -1511,10 +1492,10 @@
       <c r="D8" s="3">
         <v>129</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <v>0</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="10">
         <v>1791</v>
       </c>
       <c r="G8" s="3">
@@ -1523,7 +1504,7 @@
       <c r="H8" s="3">
         <v>44</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I8" s="14">
         <v>1</v>
       </c>
       <c r="J8" s="3">
@@ -1534,7 +1515,7 @@
         <f t="shared" si="1"/>
         <v>6245</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8" s="19">
         <f t="shared" si="2"/>
         <v>173</v>
       </c>
@@ -1556,10 +1537,10 @@
       <c r="D9" s="3">
         <v>16</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="14">
         <v>0</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="10">
         <v>1380</v>
       </c>
       <c r="G9" s="3">
@@ -1568,7 +1549,7 @@
       <c r="H9" s="3">
         <v>11</v>
       </c>
-      <c r="I9" s="25">
+      <c r="I9" s="14">
         <v>0</v>
       </c>
       <c r="J9" s="3">
@@ -1579,7 +1560,7 @@
         <f t="shared" si="1"/>
         <v>4406</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9" s="19">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
@@ -1592,19 +1573,19 @@
       <c r="A10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="10">
+      <c r="B10" s="5">
         <v>1546</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="10">
         <v>984</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="10">
         <v>129</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="14">
         <v>28</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="10">
         <v>142</v>
       </c>
       <c r="G10" s="3">
@@ -1613,7 +1594,7 @@
       <c r="H10" s="3">
         <v>68</v>
       </c>
-      <c r="I10" s="25">
+      <c r="I10" s="14">
         <v>43</v>
       </c>
       <c r="J10" s="3">
@@ -1624,7 +1605,7 @@
         <f t="shared" si="1"/>
         <v>1120</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10" s="19">
         <f t="shared" si="2"/>
         <v>197</v>
       </c>
@@ -1634,63 +1615,63 @@
       </c>
     </row>
     <row r="11" spans="1:13">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="13">
-        <f>SUM(B3:B10)</f>
+      <c r="B11" s="12">
+        <f t="shared" ref="B11:M11" si="4">SUM(B3:B10)</f>
         <v>231493</v>
       </c>
-      <c r="C11" s="14">
-        <f>SUM(C3:C10)</f>
+      <c r="C11" s="13">
+        <f t="shared" si="4"/>
         <v>204180</v>
       </c>
-      <c r="D11" s="14">
-        <f>SUM(D3:D10)</f>
+      <c r="D11" s="13">
+        <f t="shared" si="4"/>
         <v>45397</v>
       </c>
-      <c r="E11" s="20">
-        <f>SUM(E3:E10)</f>
+      <c r="E11" s="16">
+        <f t="shared" si="4"/>
         <v>11639</v>
       </c>
-      <c r="F11" s="21">
-        <f>SUM(F3:F10)</f>
+      <c r="F11" s="13">
+        <f t="shared" si="4"/>
         <v>37873</v>
       </c>
-      <c r="G11" s="14">
-        <f>SUM(G3:G10)</f>
+      <c r="G11" s="13">
+        <f t="shared" si="4"/>
         <v>35411</v>
       </c>
-      <c r="H11" s="14">
-        <f>SUM(H3:H10)</f>
+      <c r="H11" s="13">
+        <f t="shared" si="4"/>
         <v>9373</v>
       </c>
-      <c r="I11" s="27">
-        <f>SUM(I3:I10)</f>
+      <c r="I11" s="14">
+        <f t="shared" si="4"/>
         <v>2427</v>
       </c>
-      <c r="J11" s="14">
-        <f>SUM(J3:J10)</f>
+      <c r="J11" s="13">
+        <f t="shared" si="4"/>
         <v>269366</v>
       </c>
-      <c r="K11" s="14">
-        <f>SUM(K3:K10)</f>
+      <c r="K11" s="13">
+        <f t="shared" si="4"/>
         <v>239591</v>
       </c>
-      <c r="L11" s="14">
-        <f>SUM(L3:L10)</f>
+      <c r="L11" s="13">
+        <f t="shared" si="4"/>
         <v>54770</v>
       </c>
-      <c r="M11" s="31">
-        <f>SUM(M3:M10)</f>
+      <c r="M11" s="22">
+        <f t="shared" si="4"/>
         <v>14066</v>
       </c>
     </row>
     <row r="12" spans="9:9">
-      <c r="I12" s="28"/>
+      <c r="I12" s="20"/>
     </row>
     <row r="13" spans="9:9">
-      <c r="I13" s="29"/>
+      <c r="I13" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Auto commit Tue Jul  5 17:40:01 IST 2022
</commit_message>
<xml_diff>
--- a/temp_files/source-prediction-counts.xlsx
+++ b/temp_files/source-prediction-counts.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>class</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>4-sigma :</t>
   </si>
 </sst>
 </file>
@@ -1183,10 +1186,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleSheetLayoutView="60" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8" defaultRowHeight="15.75"/>
@@ -1623,7 +1626,7 @@
         <v>231493</v>
       </c>
       <c r="C11" s="13">
-        <f t="shared" si="4"/>
+        <f>SUM(C3:C10)</f>
         <v>204180</v>
       </c>
       <c r="D11" s="13">
@@ -1672,6 +1675,14 @@
     </row>
     <row r="13" spans="9:9">
       <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3">
+        <v>99.99</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>